<commit_message>
feat: seed questions and answers with xlsx
</commit_message>
<xml_diff>
--- a/database/seeders/questions.xlsx
+++ b/database/seeders/questions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin Zweifel\Documents\_HEIG-VD\MEDIA\_ProjArt\mantastudio-projart\database\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62CC2CB-43B6-4159-8958-A443F7FFA643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F34E1B8-8832-445B-BD48-46C645C5FF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{6B503C13-100F-44EA-9D5A-26E4AF0C4008}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{6B503C13-100F-44EA-9D5A-26E4AF0C4008}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
+    <sheet name="Answers" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>text</t>
   </si>
@@ -76,6 +77,24 @@
   </si>
   <si>
     <t>city_id</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>question_id</t>
+  </si>
+  <si>
+    <t>hdkjfhaf</t>
+  </si>
+  <si>
+    <t>ajfdljasfdlkjdsf</t>
+  </si>
+  <si>
+    <t>dsjflkjdsafljsalkfd</t>
+  </si>
+  <si>
+    <t>jaslfdj</t>
   </si>
 </sst>
 </file>
@@ -140,6 +159,18 @@
     <tableColumn id="4" xr3:uid="{37EC6670-876E-4242-83AA-936389B6F1D2}" name="image_dyk_url"/>
     <tableColumn id="5" xr3:uid="{9255152C-6B79-4561-ADDD-419ECF808C20}" name="question_category_id"/>
     <tableColumn id="6" xr3:uid="{112D1DB1-D276-40BA-97B6-763818599491}" name="city_id"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{10EB6697-D244-4C62-9465-C75B2B9E6063}" name="Tableau2" displayName="Tableau2" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5" xr:uid="{10EB6697-D244-4C62-9465-C75B2B9E6063}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{57D1411B-C87A-4498-ACF1-9BAFD6221C69}" name="text"/>
+    <tableColumn id="2" xr3:uid="{48120E68-4891-4893-9462-C982D56B77A1}" name="correct"/>
+    <tableColumn id="3" xr3:uid="{3E1FB5ED-C676-4E3C-BB7F-3153EDFF65DD}" name="question_id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -444,7 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E0F8DD-4129-4264-B9C9-CBE9DA74E00D}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H1:I1048576"/>
     </sheetView>
   </sheetViews>
@@ -521,4 +552,80 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B619A5A-9888-44E3-9FBC-E089F0394641}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="12.4609375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: missing question answers
</commit_message>
<xml_diff>
--- a/database/seeders/questions.xlsx
+++ b/database/seeders/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Mon Drive\HEIG-VD\2Annee\ProjArt\Réalisation\Production de Contenu\Contenu Textuel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106BF8A1-7A3D-48CE-B61A-9C61DD3B01F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACFBFC9-0263-408E-B1D6-FB9E7719BCDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="325">
   <si>
     <t>text</t>
   </si>
@@ -990,6 +990,18 @@
   </si>
   <si>
     <t>Prix nobel en mathématique</t>
+  </si>
+  <si>
+    <t>Guet de la Cathédrale</t>
+  </si>
+  <si>
+    <t>Faire pousser un palmier</t>
+  </si>
+  <si>
+    <t>Défilé militaire</t>
+  </si>
+  <si>
+    <t>Marathon de Lausanne</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1212,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:C253">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:C257">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="text"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="correct"/>
@@ -1410,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3288,8 +3300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="A261" sqref="A261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6083,25 +6095,65 @@
         <v>32</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>323</v>
+      </c>
+      <c r="B254">
+        <v>0</v>
+      </c>
+      <c r="C254">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>322</v>
+      </c>
+      <c r="B255">
+        <v>0</v>
+      </c>
+      <c r="C255">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>321</v>
+      </c>
+      <c r="B256">
+        <v>1</v>
+      </c>
+      <c r="C256">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>324</v>
+      </c>
+      <c r="B257">
+        <v>0</v>
+      </c>
+      <c r="C257">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>